<commit_message>
add recursion limit to tester and view and data to excel
</commit_message>
<xml_diff>
--- a/Docs/ISIS1225 - Tablas de Datos Lab 4-5.xlsx
+++ b/Docs/ISIS1225 - Tablas de Datos Lab 4-5.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Abel Arismendy\python_projects\Reto1-G07\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2AFA656-1913-4122-87DE-11B78304F9B4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8A38DF9-0E62-4F16-8E6C-4F7776DAEB0C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{D82936D8-D2C9-4EB2-9CBC-3665F65B95FD}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="1" activeTab="1" xr2:uid="{D82936D8-D2C9-4EB2-9CBC-3665F65B95FD}"/>
   </bookViews>
   <sheets>
     <sheet name="Datos Lab4-5" sheetId="1" r:id="rId1"/>
@@ -307,7 +307,54 @@
         <name val="Dax-Regular"/>
         <scheme val="none"/>
       </font>
-      <numFmt numFmtId="2" formatCode="0.00"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Dax-Regular"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="justify" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Dax-Regular"/>
+        <scheme val="none"/>
+      </font>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
@@ -382,54 +429,7 @@
         <name val="Dax-Regular"/>
         <scheme val="none"/>
       </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Dax-Regular"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="justify" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="Dax-Regular"/>
-        <scheme val="none"/>
-      </font>
+      <numFmt numFmtId="2" formatCode="0.00"/>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
@@ -649,7 +649,17 @@
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="9.5863764214734165E-2"/>
+          <c:y val="8.9811994503821824E-2"/>
+          <c:w val="0.87045489835776668"/>
+          <c:h val="0.8097070076271814"/>
+        </c:manualLayout>
+      </c:layout>
       <c:scatterChart>
         <c:scatterStyle val="smoothMarker"/>
         <c:varyColors val="0"/>
@@ -701,7 +711,7 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
-            <c:trendlineType val="linear"/>
+            <c:trendlineType val="power"/>
             <c:dispRSqr val="1"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
@@ -737,10 +747,10 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>'Datos Lab4-5'!$A$2:$A$11</c:f>
+              <c:f>'Datos Lab4-5'!$A$2:$A$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>1000</c:v>
                 </c:pt>
@@ -761,25 +771,16 @@
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>64000</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>128000</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>256000</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>375942</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Datos Lab4-5'!$B$2:$B$11</c:f>
+              <c:f>'Datos Lab4-5'!$B$2:$B$8</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>453.13</c:v>
                 </c:pt>
@@ -859,8 +860,7 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
-            <c:trendlineType val="poly"/>
-            <c:order val="2"/>
+            <c:trendlineType val="power"/>
             <c:dispRSqr val="1"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
@@ -896,10 +896,10 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>'Datos Lab4-5'!$A$2:$A$11</c:f>
+              <c:f>'Datos Lab4-5'!$A$2:$A$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>1000</c:v>
                 </c:pt>
@@ -920,25 +920,16 @@
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>64000</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>128000</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>256000</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>375942</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Datos Lab4-5'!$C$2:$C$11</c:f>
+              <c:f>'Datos Lab4-5'!$C$2:$C$8</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>494.79</c:v>
                 </c:pt>
@@ -1018,51 +1009,7 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
-            <c:trendlineType val="log"/>
-            <c:dispRSqr val="1"/>
-            <c:dispEq val="1"/>
-            <c:trendlineLbl>
-              <c:numFmt formatCode="General" sourceLinked="0"/>
-              <c:spPr>
-                <a:noFill/>
-                <a:ln>
-                  <a:noFill/>
-                </a:ln>
-                <a:effectLst/>
-              </c:spPr>
-              <c:txPr>
-                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-                <a:lstStyle/>
-                <a:p>
-                  <a:pPr>
-                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                      <a:solidFill>
-                        <a:schemeClr val="tx1">
-                          <a:lumMod val="65000"/>
-                          <a:lumOff val="35000"/>
-                        </a:schemeClr>
-                      </a:solidFill>
-                      <a:latin typeface="+mn-lt"/>
-                      <a:ea typeface="+mn-ea"/>
-                      <a:cs typeface="+mn-cs"/>
-                    </a:defRPr>
-                  </a:pPr>
-                  <a:endParaRPr lang="en-US"/>
-                </a:p>
-              </c:txPr>
-            </c:trendlineLbl>
-          </c:trendline>
-          <c:trendline>
-            <c:spPr>
-              <a:ln w="19050" cap="rnd">
-                <a:solidFill>
-                  <a:schemeClr val="accent4"/>
-                </a:solidFill>
-                <a:prstDash val="sysDot"/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:trendlineType val="linear"/>
+            <c:trendlineType val="power"/>
             <c:dispRSqr val="1"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
@@ -1237,7 +1184,7 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
-            <c:trendlineType val="linear"/>
+            <c:trendlineType val="power"/>
             <c:dispRSqr val="1"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
@@ -1316,6 +1263,36 @@
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>18.75</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>43.75</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>81.25</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>178.125</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>387.5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>831.25</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1843.75</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>4040.625</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>8643.75</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>13884.38</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
@@ -1382,7 +1359,7 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
-            <c:trendlineType val="linear"/>
+            <c:trendlineType val="log"/>
             <c:dispRSqr val="1"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
@@ -1461,6 +1438,36 @@
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>15.625</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>40.625</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>80.73</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>182.23</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>384.375</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>831.25</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1815.625</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3856.25</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>8340.6299999999992</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>12815.63</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
@@ -1728,7 +1735,7 @@
       </c:valAx>
       <c:spPr>
         <a:noFill/>
-        <a:ln>
+        <a:ln w="25400">
           <a:noFill/>
         </a:ln>
         <a:effectLst/>
@@ -1942,7 +1949,7 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
-            <c:trendlineType val="linear"/>
+            <c:trendlineType val="power"/>
             <c:dispRSqr val="1"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
@@ -1978,10 +1985,10 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>'Datos Lab4-5'!$A$15:$A$24</c:f>
+              <c:f>'Datos Lab4-5'!$A$15:$A$18</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
                   <c:v>1000</c:v>
                 </c:pt>
@@ -1993,34 +2000,16 @@
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>8000</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>16000</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>32000</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>64000</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>128000</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>256000</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>375942</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Datos Lab4-5'!$B$15:$B$24</c:f>
+              <c:f>'Datos Lab4-5'!$B$15:$B$19</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
                   <c:v>30921.875</c:v>
                 </c:pt>
@@ -2091,7 +2080,7 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
-            <c:trendlineType val="linear"/>
+            <c:trendlineType val="power"/>
             <c:dispRSqr val="1"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
@@ -2127,10 +2116,10 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>'Datos Lab4-5'!$A$15:$A$24</c:f>
+              <c:f>'Datos Lab4-5'!$A$15:$A$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="3"/>
                 <c:pt idx="0">
                   <c:v>1000</c:v>
                 </c:pt>
@@ -2139,37 +2128,16 @@
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>4000</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>8000</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>16000</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>32000</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>64000</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>128000</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>256000</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>375942</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Datos Lab4-5'!$C$15:$C$24</c:f>
+              <c:f>'Datos Lab4-5'!$C$15:$C$17</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="3"/>
                 <c:pt idx="0">
                   <c:v>27765.625</c:v>
                 </c:pt>
@@ -2237,7 +2205,7 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
-            <c:trendlineType val="linear"/>
+            <c:trendlineType val="power"/>
             <c:dispRSqr val="1"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
@@ -2273,10 +2241,10 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>'Datos Lab4-5'!$A$15:$A$24</c:f>
+              <c:f>'Datos Lab4-5'!$A$15:$A$19</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
                   <c:v>1000</c:v>
                 </c:pt>
@@ -2291,31 +2259,16 @@
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>16000</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>32000</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>64000</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>128000</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>256000</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>375942</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Datos Lab4-5'!$D$15:$D$24</c:f>
+              <c:f>'Datos Lab4-5'!$D$15:$D$19</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
                   <c:v>1640.625</c:v>
                 </c:pt>
@@ -2397,7 +2350,7 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
-            <c:trendlineType val="linear"/>
+            <c:trendlineType val="power"/>
             <c:dispRSqr val="1"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
@@ -2433,10 +2386,10 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>'Datos Lab4-5'!$A$15:$A$24</c:f>
+              <c:f>'Datos Lab4-5'!$A$15:$A$21</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>1000</c:v>
                 </c:pt>
@@ -2457,25 +2410,37 @@
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>64000</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>128000</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>256000</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>375942</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Datos Lab4-5'!$E$15:$E$24</c:f>
+              <c:f>'Datos Lab4-5'!$E$15:$E$21</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>1343.75</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6005.2079999999996</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>23765.63</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>104349</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>448984.4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1904281</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>8351094</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
@@ -2542,7 +2507,7 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
-            <c:trendlineType val="linear"/>
+            <c:trendlineType val="power"/>
             <c:dispRSqr val="1"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
@@ -2578,10 +2543,10 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>'Datos Lab4-5'!$A$15:$A$24</c:f>
+              <c:f>'Datos Lab4-5'!$A$15:$A$21</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>1000</c:v>
                 </c:pt>
@@ -2602,25 +2567,34 @@
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>64000</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>128000</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>256000</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>375942</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Datos Lab4-5'!$F$15:$F$24</c:f>
+              <c:f>'Datos Lab4-5'!$F$15:$F$21</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>191.4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>613.28</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2421.88</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>9566.4060000000009</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>38117.19</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>153593.79999999999</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
@@ -3092,7 +3066,7 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
-            <c:trendlineType val="linear"/>
+            <c:trendlineType val="power"/>
             <c:dispRSqr val="1"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
@@ -3128,10 +3102,10 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>'Datos Lab4-5'!$A$2:$A$11</c:f>
+              <c:f>'Datos Lab4-5'!$A$2:$A$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>1000</c:v>
                 </c:pt>
@@ -3152,25 +3126,16 @@
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>64000</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>128000</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>256000</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>375942</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Datos Lab4-5'!$B$2:$B$11</c:f>
+              <c:f>'Datos Lab4-5'!$B$2:$B$8</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>453.13</c:v>
                 </c:pt>
@@ -3250,7 +3215,7 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
-            <c:trendlineType val="linear"/>
+            <c:trendlineType val="power"/>
             <c:dispRSqr val="1"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
@@ -3286,10 +3251,10 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>'Datos Lab4-5'!$A$15:$A$24</c:f>
+              <c:f>'Datos Lab4-5'!$A$15:$A$18</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
                   <c:v>1000</c:v>
                 </c:pt>
@@ -3301,34 +3266,16 @@
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>8000</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>16000</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>32000</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>64000</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>128000</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>256000</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>375942</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Datos Lab4-5'!$B$15:$B$24</c:f>
+              <c:f>'Datos Lab4-5'!$B$15:$B$18</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
                   <c:v>30921.875</c:v>
                 </c:pt>
@@ -3802,7 +3749,7 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
-            <c:trendlineType val="linear"/>
+            <c:trendlineType val="power"/>
             <c:dispRSqr val="1"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
@@ -3838,10 +3785,10 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>'Datos Lab4-5'!$A$2:$A$11</c:f>
+              <c:f>'Datos Lab4-5'!$A$2:$A$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>1000</c:v>
                 </c:pt>
@@ -3862,25 +3809,16 @@
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>64000</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>128000</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>256000</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>375942</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Datos Lab4-5'!$C$2:$C$11</c:f>
+              <c:f>'Datos Lab4-5'!$C$2:$C$8</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>494.79</c:v>
                 </c:pt>
@@ -3960,7 +3898,7 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
-            <c:trendlineType val="linear"/>
+            <c:trendlineType val="power"/>
             <c:dispRSqr val="1"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
@@ -3996,10 +3934,10 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>'Datos Lab4-5'!$A$15:$A$24</c:f>
+              <c:f>'Datos Lab4-5'!$A$15:$A$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="3"/>
                 <c:pt idx="0">
                   <c:v>1000</c:v>
                 </c:pt>
@@ -4008,37 +3946,16 @@
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>4000</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>8000</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>16000</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>32000</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>64000</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>128000</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>256000</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>375942</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Datos Lab4-5'!$C$15:$C$24</c:f>
+              <c:f>'Datos Lab4-5'!$C$15:$C$17</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="3"/>
                 <c:pt idx="0">
                   <c:v>27765.625</c:v>
                 </c:pt>
@@ -4509,7 +4426,8 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
-            <c:trendlineType val="linear"/>
+            <c:trendlineType val="poly"/>
+            <c:order val="2"/>
             <c:dispRSqr val="1"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
@@ -4676,7 +4594,7 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
-            <c:trendlineType val="linear"/>
+            <c:trendlineType val="power"/>
             <c:dispRSqr val="1"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
@@ -4712,10 +4630,10 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>'Datos Lab4-5'!$A$15:$A$24</c:f>
+              <c:f>'Datos Lab4-5'!$A$15:$A$19</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
                   <c:v>1000</c:v>
                 </c:pt>
@@ -4730,31 +4648,16 @@
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>16000</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>32000</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>64000</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>128000</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>256000</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>375942</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Datos Lab4-5'!$D$15:$D$24</c:f>
+              <c:f>'Datos Lab4-5'!$D$15:$D$19</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
                   <c:v>1640.625</c:v>
                 </c:pt>
@@ -5187,7 +5090,17 @@
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.11940873893704258"/>
+          <c:y val="7.7511059127311738E-2"/>
+          <c:w val="0.84554016207274973"/>
+          <c:h val="0.78188980381619078"/>
+        </c:manualLayout>
+      </c:layout>
       <c:scatterChart>
         <c:scatterStyle val="smoothMarker"/>
         <c:varyColors val="0"/>
@@ -5239,7 +5152,7 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
-            <c:trendlineType val="linear"/>
+            <c:trendlineType val="power"/>
             <c:dispRSqr val="1"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
@@ -5318,6 +5231,36 @@
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>18.75</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>43.75</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>81.25</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>178.125</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>387.5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>831.25</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1843.75</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>4040.625</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>8643.75</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>13884.38</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
@@ -5376,7 +5319,7 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
-            <c:trendlineType val="linear"/>
+            <c:trendlineType val="power"/>
             <c:dispRSqr val="1"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
@@ -5412,10 +5355,10 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>'Datos Lab4-5'!$A$15:$A$24</c:f>
+              <c:f>'Datos Lab4-5'!$A$15:$A$21</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>1000</c:v>
                 </c:pt>
@@ -5436,25 +5379,37 @@
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>64000</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>128000</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>256000</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>375942</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Datos Lab4-5'!$E$15:$E$24</c:f>
+              <c:f>'Datos Lab4-5'!$E$15:$E$21</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>1343.75</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6005.2079999999996</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>23765.63</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>104349</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>448984.4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1904281</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>8351094</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
@@ -5924,8 +5879,7 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
-            <c:trendlineType val="poly"/>
-            <c:order val="2"/>
+            <c:trendlineType val="power"/>
             <c:dispRSqr val="1"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
@@ -6004,6 +5958,36 @@
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>15.625</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>40.625</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>80.73</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>182.23</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>384.375</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>831.25</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1815.625</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3856.25</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>8340.6299999999992</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>12815.63</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
@@ -6062,8 +6046,7 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
-            <c:trendlineType val="poly"/>
-            <c:order val="2"/>
+            <c:trendlineType val="power"/>
             <c:dispRSqr val="1"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
@@ -6099,10 +6082,10 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>'Datos Lab4-5'!$A$15:$A$24</c:f>
+              <c:f>'Datos Lab4-5'!$A$15:$A$21</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>1000</c:v>
                 </c:pt>
@@ -6123,25 +6106,34 @@
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>64000</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>128000</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>256000</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>375942</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Datos Lab4-5'!$F$15:$F$24</c:f>
+              <c:f>'Datos Lab4-5'!$F$15:$F$21</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>191.4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>613.28</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2421.88</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>9566.4060000000009</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>38117.19</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>153593.79999999999</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
@@ -10370,7 +10362,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{BF2A59F4-6CD8-490D-818C-7B3BB3F2B140}">
   <sheetPr/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="115" workbookViewId="0"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -10679,26 +10671,26 @@
   <autoFilter ref="A1:F11" xr:uid="{B245DDE7-54F2-4A7A-AC17-5CA17DD7B03F}"/>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{A7AF2A2F-BC4B-404E-9B8B-256DA178E68B}" name="Tamaño de la muestra (ARRAYLIST)" dataDxfId="13"/>
-    <tableColumn id="2" xr3:uid="{23CECC62-35E0-466E-9502-4F5CC2E6F7A7}" name="Insertion Sort [ms]" dataDxfId="5"/>
-    <tableColumn id="3" xr3:uid="{19B1D273-887B-4392-991E-015D36D99E5B}" name="Selection Sort [ms]" dataDxfId="4"/>
-    <tableColumn id="4" xr3:uid="{56471E76-DCC6-4EED-8237-BCC256B57E91}" name="Shell Sort [ms]" dataDxfId="3"/>
-    <tableColumn id="5" xr3:uid="{61DF25D7-A2A3-4D39-B0C6-29804C1B33DB}" name="Quick Sort [ms]" dataDxfId="12"/>
-    <tableColumn id="6" xr3:uid="{6FC8F4B7-6274-4B14-98D8-0E00E479351A}" name="Merge Sort [ms]" dataDxfId="11"/>
+    <tableColumn id="2" xr3:uid="{23CECC62-35E0-466E-9502-4F5CC2E6F7A7}" name="Insertion Sort [ms]" dataDxfId="12"/>
+    <tableColumn id="3" xr3:uid="{19B1D273-887B-4392-991E-015D36D99E5B}" name="Selection Sort [ms]" dataDxfId="11"/>
+    <tableColumn id="4" xr3:uid="{56471E76-DCC6-4EED-8237-BCC256B57E91}" name="Shell Sort [ms]" dataDxfId="10"/>
+    <tableColumn id="5" xr3:uid="{61DF25D7-A2A3-4D39-B0C6-29804C1B33DB}" name="Quick Sort [ms]" dataDxfId="9"/>
+    <tableColumn id="6" xr3:uid="{6FC8F4B7-6274-4B14-98D8-0E00E479351A}" name="Merge Sort [ms]" dataDxfId="8"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{C35EFFA4-2B65-46C5-8257-6884800B9577}" name="Table13" displayName="Table13" ref="A14:F24" totalsRowShown="0" headerRowDxfId="10" dataDxfId="9">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{C35EFFA4-2B65-46C5-8257-6884800B9577}" name="Table13" displayName="Table13" ref="A14:F24" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
   <autoFilter ref="A14:F24" xr:uid="{5C24B5A8-1B8E-4092-B34A-66FF5413D106}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{16584851-71BC-4FF5-B248-C3F46BA653AF}" name="Tamaño de la muestra (LINKED_LIST)" dataDxfId="8"/>
-    <tableColumn id="2" xr3:uid="{4F9B7329-040C-4D35-96E7-B9181424DC65}" name="Insertion Sort [ms]" dataDxfId="2"/>
-    <tableColumn id="3" xr3:uid="{BDA028DF-4CED-4928-B040-96AD8F8A43EB}" name="Selection Sort [ms]" dataDxfId="1"/>
-    <tableColumn id="4" xr3:uid="{A5E99D51-DD73-48A7-AE0D-601A8EE89AFA}" name="Shell Sort [ms]" dataDxfId="0"/>
-    <tableColumn id="5" xr3:uid="{EE99E4CD-A6F0-492B-B754-38221659D42F}" name="Quick Sort [ms]" dataDxfId="7"/>
-    <tableColumn id="6" xr3:uid="{21628D13-D0BA-41D1-8E51-AB02437FBDE5}" name="Merge Sort [ms]" dataDxfId="6"/>
+    <tableColumn id="1" xr3:uid="{16584851-71BC-4FF5-B248-C3F46BA653AF}" name="Tamaño de la muestra (LINKED_LIST)" dataDxfId="5"/>
+    <tableColumn id="2" xr3:uid="{4F9B7329-040C-4D35-96E7-B9181424DC65}" name="Insertion Sort [ms]" dataDxfId="4"/>
+    <tableColumn id="3" xr3:uid="{BDA028DF-4CED-4928-B040-96AD8F8A43EB}" name="Selection Sort [ms]" dataDxfId="3"/>
+    <tableColumn id="4" xr3:uid="{A5E99D51-DD73-48A7-AE0D-601A8EE89AFA}" name="Shell Sort [ms]" dataDxfId="2"/>
+    <tableColumn id="5" xr3:uid="{EE99E4CD-A6F0-492B-B754-38221659D42F}" name="Quick Sort [ms]" dataDxfId="1"/>
+    <tableColumn id="6" xr3:uid="{21628D13-D0BA-41D1-8E51-AB02437FBDE5}" name="Merge Sort [ms]" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -11001,10 +10993,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5B14742-4EBB-4241-AC8A-0E5F24F7BB7B}">
-  <dimension ref="A1:F24"/>
+  <dimension ref="A1:I24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H23" sqref="H23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -11016,7 +11008,7 @@
     <col min="5" max="6" width="22.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:9">
       <c r="A1" s="2" t="s">
         <v>4</v>
       </c>
@@ -11036,7 +11028,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:9">
       <c r="A2" s="1">
         <v>1000</v>
       </c>
@@ -11049,10 +11041,14 @@
       <c r="D2" s="6">
         <v>56.25</v>
       </c>
-      <c r="E2" s="5"/>
-      <c r="F2" s="5"/>
+      <c r="E2" s="5">
+        <v>18.75</v>
+      </c>
+      <c r="F2" s="5">
+        <v>15.625</v>
+      </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:9">
       <c r="A3" s="1">
         <v>2000</v>
       </c>
@@ -11065,10 +11061,17 @@
       <c r="D3" s="6">
         <v>71.88</v>
       </c>
-      <c r="E3" s="5"/>
-      <c r="F3" s="5"/>
+      <c r="E3" s="5">
+        <v>43.75</v>
+      </c>
+      <c r="F3" s="5">
+        <v>40.625</v>
+      </c>
+      <c r="I3">
+        <v>153406.25</v>
+      </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:9">
       <c r="A4" s="1">
         <v>4000</v>
       </c>
@@ -11081,10 +11084,17 @@
       <c r="D4" s="6">
         <v>150</v>
       </c>
-      <c r="E4" s="5"/>
-      <c r="F4" s="5"/>
+      <c r="E4" s="5">
+        <v>81.25</v>
+      </c>
+      <c r="F4" s="5">
+        <v>80.73</v>
+      </c>
+      <c r="I4">
+        <v>153781.25</v>
+      </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:9">
       <c r="A5" s="1">
         <v>8000</v>
       </c>
@@ -11097,10 +11107,14 @@
       <c r="D5" s="6">
         <v>312.5</v>
       </c>
-      <c r="E5" s="5"/>
-      <c r="F5" s="5"/>
+      <c r="E5" s="5">
+        <v>178.125</v>
+      </c>
+      <c r="F5" s="5">
+        <v>182.23</v>
+      </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:9">
       <c r="A6" s="1">
         <v>16000</v>
       </c>
@@ -11113,10 +11127,14 @@
       <c r="D6" s="6">
         <v>721.88</v>
       </c>
-      <c r="E6" s="5"/>
-      <c r="F6" s="5"/>
+      <c r="E6" s="5">
+        <v>387.5</v>
+      </c>
+      <c r="F6" s="5">
+        <v>384.375</v>
+      </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:9">
       <c r="A7" s="1">
         <v>32000</v>
       </c>
@@ -11129,10 +11147,14 @@
       <c r="D7" s="6">
         <v>1531.25</v>
       </c>
-      <c r="E7" s="5"/>
-      <c r="F7" s="5"/>
+      <c r="E7" s="5">
+        <v>831.25</v>
+      </c>
+      <c r="F7" s="5">
+        <v>831.25</v>
+      </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:9">
       <c r="A8" s="1">
         <v>64000</v>
       </c>
@@ -11145,10 +11167,14 @@
       <c r="D8" s="6">
         <v>3818.75</v>
       </c>
-      <c r="E8" s="5"/>
-      <c r="F8" s="5"/>
+      <c r="E8" s="5">
+        <v>1843.75</v>
+      </c>
+      <c r="F8" s="5">
+        <v>1815.625</v>
+      </c>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:9">
       <c r="A9" s="1">
         <v>128000</v>
       </c>
@@ -11157,10 +11183,18 @@
       <c r="D9" s="6">
         <v>9302.08</v>
       </c>
-      <c r="E9" s="5"/>
-      <c r="F9" s="5"/>
+      <c r="E9" s="5">
+        <v>4040.625</v>
+      </c>
+      <c r="F9" s="5">
+        <v>3856.25</v>
+      </c>
+      <c r="I9">
+        <f>AVERAGE(I3:I8)</f>
+        <v>153593.75</v>
+      </c>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:9">
       <c r="A10" s="1">
         <v>256000</v>
       </c>
@@ -11169,10 +11203,14 @@
       <c r="D10" s="6">
         <v>22703</v>
       </c>
-      <c r="E10" s="5"/>
-      <c r="F10" s="5"/>
+      <c r="E10" s="5">
+        <v>8643.75</v>
+      </c>
+      <c r="F10" s="5">
+        <v>8340.6299999999992</v>
+      </c>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:9">
       <c r="A11" s="7">
         <v>375942</v>
       </c>
@@ -11181,10 +11219,14 @@
       <c r="D11" s="6">
         <v>36390.625</v>
       </c>
-      <c r="E11" s="5"/>
-      <c r="F11" s="5"/>
+      <c r="E11" s="5">
+        <v>13884.38</v>
+      </c>
+      <c r="F11" s="5">
+        <v>12815.63</v>
+      </c>
     </row>
-    <row r="14" spans="1:6">
+    <row r="14" spans="1:9">
       <c r="A14" s="2" t="s">
         <v>0</v>
       </c>
@@ -11204,7 +11246,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="15" spans="1:6">
+    <row r="15" spans="1:9">
       <c r="A15" s="1">
         <v>1000</v>
       </c>
@@ -11217,10 +11259,14 @@
       <c r="D15" s="6">
         <v>1640.625</v>
       </c>
-      <c r="E15" s="5"/>
-      <c r="F15" s="5"/>
+      <c r="E15" s="5">
+        <v>1343.75</v>
+      </c>
+      <c r="F15" s="5">
+        <v>191.4</v>
+      </c>
     </row>
-    <row r="16" spans="1:6">
+    <row r="16" spans="1:9">
       <c r="A16" s="1">
         <v>2000</v>
       </c>
@@ -11233,8 +11279,12 @@
       <c r="D16" s="6">
         <v>6875</v>
       </c>
-      <c r="E16" s="5"/>
-      <c r="F16" s="5"/>
+      <c r="E16" s="5">
+        <v>6005.2079999999996</v>
+      </c>
+      <c r="F16" s="5">
+        <v>613.28</v>
+      </c>
     </row>
     <row r="17" spans="1:6">
       <c r="A17" s="1">
@@ -11249,8 +11299,12 @@
       <c r="D17" s="6">
         <v>33000</v>
       </c>
-      <c r="E17" s="5"/>
-      <c r="F17" s="5"/>
+      <c r="E17" s="5">
+        <v>23765.63</v>
+      </c>
+      <c r="F17" s="5">
+        <v>2421.88</v>
+      </c>
     </row>
     <row r="18" spans="1:6">
       <c r="A18" s="1">
@@ -11263,8 +11317,12 @@
       <c r="D18" s="6">
         <v>173265.625</v>
       </c>
-      <c r="E18" s="5"/>
-      <c r="F18" s="5"/>
+      <c r="E18" s="5">
+        <v>104349</v>
+      </c>
+      <c r="F18" s="5">
+        <v>9566.4060000000009</v>
+      </c>
     </row>
     <row r="19" spans="1:6">
       <c r="A19" s="1">
@@ -11275,8 +11333,12 @@
       <c r="D19" s="6">
         <v>798406.25</v>
       </c>
-      <c r="E19" s="5"/>
-      <c r="F19" s="5"/>
+      <c r="E19" s="5">
+        <v>448984.4</v>
+      </c>
+      <c r="F19" s="5">
+        <v>38117.19</v>
+      </c>
     </row>
     <row r="20" spans="1:6">
       <c r="A20" s="1">
@@ -11285,8 +11347,12 @@
       <c r="B20" s="4"/>
       <c r="C20" s="4"/>
       <c r="D20" s="4"/>
-      <c r="E20" s="5"/>
-      <c r="F20" s="5"/>
+      <c r="E20" s="5">
+        <v>1904281</v>
+      </c>
+      <c r="F20" s="5">
+        <v>153593.79999999999</v>
+      </c>
     </row>
     <row r="21" spans="1:6">
       <c r="A21" s="1">
@@ -11295,7 +11361,9 @@
       <c r="B21" s="4"/>
       <c r="C21" s="4"/>
       <c r="D21" s="4"/>
-      <c r="E21" s="5"/>
+      <c r="E21" s="5">
+        <v>8351094</v>
+      </c>
       <c r="F21" s="5"/>
     </row>
     <row r="22" spans="1:6">

</xml_diff>